<commit_message>
updating Pagefactory Model framework
</commit_message>
<xml_diff>
--- a/Home1/TestData.xlsx
+++ b/Home1/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -16,15 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>UserName</t>
   </si>
   <si>
     <t>Password</t>
-  </si>
-  <si>
-    <t>kame9454</t>
   </si>
   <si>
     <t>km275101@gmail.com</t>
@@ -415,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -431,10 +428,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
         <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1234</v>
       </c>
     </row>
   </sheetData>
@@ -449,70 +446,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>